<commit_message>
Included statisical analysis results for number of days non-depressed patients measured their activity in Excel
</commit_message>
<xml_diff>
--- a/results/Statistical Analysis Results.xlsx
+++ b/results/Statistical Analysis Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazia\Desktop\Python Udemy\GitRepo\CS3IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2146441-8527-4A23-93B1-41BD78AC79B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA5189A-C7BF-40F4-9D0F-6AD9AD7EEFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E472CA01-CCAC-4AD8-8CA7-118BF969A029}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{E472CA01-CCAC-4AD8-8CA7-118BF969A029}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Number of days</t>
   </si>
@@ -74,7 +74,19 @@
     <t>Variance</t>
   </si>
   <si>
-    <t>MADRS Score for Depressed Patients</t>
+    <t>MADRS Scores</t>
+  </si>
+  <si>
+    <t>Start (madrs1)</t>
+  </si>
+  <si>
+    <t>End (madrs2)</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>MADRS Score for Depressed Patients (Condition)</t>
   </si>
 </sst>
 </file>
@@ -147,11 +159,11 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -489,7 +501,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191D3949-E431-43F6-9DEC-5A58F29EDA19}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:F1"/>
@@ -497,115 +509,129 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>12.6</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>13</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>13</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>5</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>20</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>2.5</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>6.2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>12.7</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>13</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>13</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>5</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>18</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>2.8</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>7.7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="B5" s="1">
+        <v>12.6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5.4</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
+      <c r="A8" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -614,40 +640,66 @@
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Included statistical analysis results for MADRS scores in depressed patients
</commit_message>
<xml_diff>
--- a/results/Statistical Analysis Results.xlsx
+++ b/results/Statistical Analysis Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazia\Desktop\Python Udemy\GitRepo\CS3IP\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA5189A-C7BF-40F4-9D0F-6AD9AD7EEFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A04EBE4-1F73-4F20-93CB-7ED5F907EEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{E472CA01-CCAC-4AD8-8CA7-118BF969A029}"/>
   </bookViews>
@@ -83,10 +83,10 @@
     <t>End (madrs2)</t>
   </si>
   <si>
-    <t>Difference</t>
-  </si>
-  <si>
     <t>MADRS Score for Depressed Patients (Condition)</t>
+  </si>
+  <si>
+    <t>24, 26</t>
   </si>
 </sst>
 </file>
@@ -157,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -165,6 +165,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -555,25 +559,25 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="6">
         <v>12.6</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="6">
         <v>13</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="6">
         <v>13</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="6">
         <v>5</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="6">
         <v>20</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="6">
         <v>2.5</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="6">
         <v>6.2</v>
       </c>
     </row>
@@ -581,25 +585,25 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="6">
         <v>12.7</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
         <v>13</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="6">
         <v>13</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="6">
         <v>5</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="6">
         <v>18</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="6">
         <v>2.8</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="6">
         <v>7.7</v>
       </c>
     </row>
@@ -607,31 +611,31 @@
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="6">
         <v>12.6</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="6">
         <v>13</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="6">
         <v>13</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="6">
         <v>8</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="6">
         <v>20</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="6">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="6">
         <v>5.4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -669,38 +673,55 @@
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="B10" s="6">
+        <v>22.7</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="6">
+        <v>24</v>
+      </c>
+      <c r="E10" s="6">
+        <v>13</v>
+      </c>
+      <c r="F10" s="6">
+        <v>29</v>
+      </c>
+      <c r="G10" s="6">
+        <v>4.8</v>
+      </c>
+      <c r="H10" s="6">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
+      <c r="B11" s="6">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6">
+        <v>21</v>
+      </c>
+      <c r="D11" s="6">
+        <v>21</v>
+      </c>
+      <c r="E11" s="6">
+        <v>11</v>
+      </c>
+      <c r="F11" s="6">
+        <v>28</v>
+      </c>
+      <c r="G11" s="6">
+        <v>4.7</v>
+      </c>
+      <c r="H11" s="6">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:F1"/>

</xml_diff>